<commit_message>
Added Class Diagram, Use Case Diagram, Project Tracker
</commit_message>
<xml_diff>
--- a/Project tracker Updated.xlsx
+++ b/Project tracker Updated.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A9C891-E717-4EC8-88FE-A027110D3E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBB0C44-9777-4D88-BFB3-4075E15035BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project tracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Category</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Student 2</t>
-  </si>
-  <si>
-    <t>Student 5</t>
   </si>
   <si>
     <t>Task Number</t>
@@ -1522,7 +1519,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1637,13 +1634,13 @@
     <row r="5" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="25">
         <v>45604</v>
@@ -1660,18 +1657,18 @@
       </c>
       <c r="I5" s="25">
         <f ca="1">TODAY()-65</f>
-        <v>45531</v>
+        <v>45534</v>
       </c>
       <c r="J5" s="25">
         <f ca="1">TODAY()</f>
-        <v>45596</v>
+        <v>45599</v>
       </c>
       <c r="K5" s="18">
         <v>5</v>
       </c>
       <c r="L5" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$I5,'Project tracker'!$J5)&lt;&gt;2,"",DAYS360('Project tracker'!$I5,'Project tracker'!$J5,FALSE))</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M5" s="18"/>
       <c r="N5" s="3"/>
@@ -1679,13 +1676,13 @@
     <row r="6" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>35</v>
       </c>
       <c r="E6" s="25">
         <v>45619</v>
@@ -1702,11 +1699,11 @@
       </c>
       <c r="I6" s="25">
         <f ca="1">TODAY()-41</f>
-        <v>45555</v>
+        <v>45558</v>
       </c>
       <c r="J6" s="25">
         <f ca="1">TODAY()-7</f>
-        <v>45589</v>
+        <v>45592</v>
       </c>
       <c r="K6" s="18">
         <v>6</v>
@@ -1721,13 +1718,13 @@
     <row r="7" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="25">
         <v>45604</v>
@@ -1744,11 +1741,11 @@
       </c>
       <c r="I7" s="25">
         <f ca="1">TODAY()-100</f>
-        <v>45496</v>
+        <v>45499</v>
       </c>
       <c r="J7" s="25">
         <f ca="1">TODAY()-27</f>
-        <v>45569</v>
+        <v>45572</v>
       </c>
       <c r="K7" s="18">
         <v>4</v>
@@ -1763,13 +1760,13 @@
     <row r="8" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="25">
         <v>45619</v>
@@ -1786,11 +1783,11 @@
       </c>
       <c r="I8" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45506</v>
+        <v>45509</v>
       </c>
       <c r="J8" s="25">
         <f ca="1">TODAY()-71</f>
-        <v>45525</v>
+        <v>45528</v>
       </c>
       <c r="K8" s="18">
         <v>1</v>
@@ -1805,13 +1802,13 @@
     <row r="9" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E9" s="25">
         <v>45607</v>
@@ -1828,11 +1825,11 @@
       </c>
       <c r="I9" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45506</v>
+        <v>45509</v>
       </c>
       <c r="J9" s="25">
         <f ca="1">TODAY()-44</f>
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="K9" s="18">
         <v>1</v>
@@ -1847,13 +1844,13 @@
     <row r="10" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="25">
         <f>E7</f>
@@ -1872,11 +1869,11 @@
       </c>
       <c r="I10" s="25">
         <f ca="1">TODAY()-60</f>
-        <v>45536</v>
+        <v>45539</v>
       </c>
       <c r="J10" s="25">
         <f ca="1">TODAY()-45</f>
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="K10" s="18">
         <v>6</v>
@@ -1891,13 +1888,13 @@
     <row r="11" spans="1:14" s="5" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="25">
         <v>45619</v>
@@ -1915,11 +1912,11 @@
       </c>
       <c r="I11" s="25">
         <f ca="1">TODAY()-44</f>
-        <v>45552</v>
+        <v>45555</v>
       </c>
       <c r="J11" s="25">
         <f ca="1">TODAY()-15</f>
-        <v>45581</v>
+        <v>45584</v>
       </c>
       <c r="K11" s="18">
         <v>5</v>
@@ -1944,26 +1941,26 @@
       </c>
       <c r="E12" s="25">
         <f ca="1">TODAY()-39</f>
-        <v>45557</v>
+        <v>45560</v>
       </c>
       <c r="F12" s="25">
         <f ca="1">TODAY()</f>
-        <v>45596</v>
+        <v>45599</v>
       </c>
       <c r="G12" s="18">
         <v>1</v>
       </c>
       <c r="H12" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E12,'Project tracker'!$F12)&lt;&gt;2,"",DAYS360('Project tracker'!$E12,'Project tracker'!$F12,FALSE))</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="25">
         <f ca="1">TODAY()-45</f>
-        <v>45551</v>
+        <v>45554</v>
       </c>
       <c r="J12" s="25">
         <f ca="1">TODAY()-5</f>
-        <v>45591</v>
+        <v>45594</v>
       </c>
       <c r="K12" s="18">
         <v>7</v>
@@ -1988,26 +1985,26 @@
       </c>
       <c r="E13" s="25">
         <f ca="1">TODAY()-95</f>
-        <v>45501</v>
+        <v>45504</v>
       </c>
       <c r="F13" s="25">
         <f ca="1">TODAY()-75</f>
-        <v>45521</v>
+        <v>45524</v>
       </c>
       <c r="G13" s="18">
         <v>1</v>
       </c>
       <c r="H13" s="21">
         <f ca="1">IF(COUNTA('Project tracker'!$E13,'Project tracker'!$F13)&lt;&gt;2,"",DAYS360('Project tracker'!$E13,'Project tracker'!$F13,FALSE))</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I13" s="25">
         <f ca="1">TODAY()-90</f>
-        <v>45506</v>
+        <v>45509</v>
       </c>
       <c r="J13" s="25">
         <f ca="1">TODAY()-80</f>
-        <v>45516</v>
+        <v>45519</v>
       </c>
       <c r="K13" s="18">
         <v>7</v>
@@ -2096,13 +2093,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2179,40 +2176,40 @@
     <row r="5" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="13"/>
     </row>
@@ -2222,7 +2219,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="13"/>
     </row>
@@ -2232,7 +2229,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="13"/>
     </row>
@@ -2258,6 +2255,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2569,36 +2595,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9066C173-72E5-4455-ACFB-9A7596D30A2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D99023F8-0F96-4650-8DC3-63EE0BD6CB59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2619,26 +2636,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648F31BC-5AA3-42BF-80F4-A797E59C4FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9066C173-72E5-4455-ACFB-9A7596D30A2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>